<commit_message>
Se implementa una interfaz por console en DemoStrategy Se actualizan unos Excel con graficos de resultados
</commit_message>
<xml_diff>
--- a/tp2/resultados/fileScan2Times.xlsx
+++ b/tp2/resultados/fileScan2Times.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="8">
   <si>
     <t>#FRAMES</t>
   </si>
@@ -29,13 +29,33 @@
   <si>
     <t>FIFO</t>
   </si>
+  <si>
+    <t>fileScan2Times.txt</t>
+  </si>
+  <si>
+    <t>LRUReplacementStrategy</t>
+  </si>
+  <si>
+    <t>MRUReplacementStrategy</t>
+  </si>
+  <si>
+    <t>FIFOReplacementStrategy</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+  <fonts count="2">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -63,9 +83,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -101,9 +122,9 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="0.12141740791315186"/>
-          <c:y val="3.9058996253436659E-2"/>
+          <c:y val="3.9058996253436652E-2"/>
           <c:w val="0.75458577402297966"/>
-          <c:h val="0.77207238277273393"/>
+          <c:h val="0.77207238277273382"/>
         </c:manualLayout>
       </c:layout>
       <c:line3DChart>
@@ -355,13 +376,12 @@
           </c:val>
           <c:bubble3D val="1"/>
         </c:ser>
-        <c:dLbls/>
-        <c:axId val="69686784"/>
-        <c:axId val="79164160"/>
-        <c:axId val="100932672"/>
+        <c:axId val="79075200"/>
+        <c:axId val="53616640"/>
+        <c:axId val="79054144"/>
       </c:line3DChart>
       <c:catAx>
-        <c:axId val="69686784"/>
+        <c:axId val="79075200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -387,14 +407,14 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="79164160"/>
+        <c:crossAx val="53616640"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="79164160"/>
+        <c:axId val="53616640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -420,12 +440,12 @@
         </c:title>
         <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="69686784"/>
+        <c:crossAx val="79075200"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:serAx>
-        <c:axId val="100932672"/>
+        <c:axId val="79054144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -433,7 +453,8 @@
         <c:axPos val="b"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="79164160"/>
+        <c:crossAx val="53616640"/>
+        <c:crosses val="autoZero"/>
       </c:serAx>
     </c:plotArea>
     <c:legend>
@@ -442,6 +463,194 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="span"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="es-AR"/>
+  <c:chart>
+    <c:view3D>
+      <c:rotX val="20"/>
+      <c:rotY val="10"/>
+      <c:perspective val="0"/>
+    </c:view3D>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.13138511651828899"/>
+          <c:y val="4.824724999262732E-2"/>
+          <c:w val="0.74695436009845584"/>
+          <c:h val="0.86941307617446695"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:line3DChart>
+        <c:grouping val="standard"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>FIFO</c:v>
+          </c:tx>
+          <c:val>
+            <c:numRef>
+              <c:f>Hoja1!$D$11:$D$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0.21</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.21</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.42</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>LRU</c:v>
+          </c:tx>
+          <c:val>
+            <c:numRef>
+              <c:f>Hoja1!$D$18:$D$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>MRU</c:v>
+          </c:tx>
+          <c:val>
+            <c:numRef>
+              <c:f>Hoja1!$D$25:$D$31</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0.28000000000000003</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.35</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.42</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:axId val="74438528"/>
+        <c:axId val="74461952"/>
+        <c:axId val="80919616"/>
+      </c:line3DChart>
+      <c:catAx>
+        <c:axId val="74438528"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="74461952"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="74461952"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="74438528"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:serAx>
+        <c:axId val="80919616"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="74461952"/>
+      </c:serAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
@@ -455,15 +664,15 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>962025</xdr:colOff>
-      <xdr:row>1</xdr:row>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>4</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>28575</xdr:colOff>
-      <xdr:row>23</xdr:row>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>685800</xdr:colOff>
+      <xdr:row>26</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -478,6 +687,36 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>733424</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>761999</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="3 Gráfico"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -784,10 +1023,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N22" sqref="N22"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -908,7 +1147,305 @@
         <v>0.5</v>
       </c>
     </row>
+    <row r="11" spans="1:4">
+      <c r="A11" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11">
+        <v>4</v>
+      </c>
+      <c r="C11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11">
+        <v>0.21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" t="s">
+        <v>4</v>
+      </c>
+      <c r="B12">
+        <v>5</v>
+      </c>
+      <c r="C12" t="s">
+        <v>7</v>
+      </c>
+      <c r="D12">
+        <v>0.21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" t="s">
+        <v>4</v>
+      </c>
+      <c r="B13">
+        <v>6</v>
+      </c>
+      <c r="C13" t="s">
+        <v>7</v>
+      </c>
+      <c r="D13">
+        <v>0.42</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" t="s">
+        <v>4</v>
+      </c>
+      <c r="B14">
+        <v>7</v>
+      </c>
+      <c r="C14" t="s">
+        <v>7</v>
+      </c>
+      <c r="D14">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" t="s">
+        <v>4</v>
+      </c>
+      <c r="B15">
+        <v>8</v>
+      </c>
+      <c r="C15" t="s">
+        <v>7</v>
+      </c>
+      <c r="D15">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B16">
+        <v>9</v>
+      </c>
+      <c r="C16" t="s">
+        <v>7</v>
+      </c>
+      <c r="D16">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" t="s">
+        <v>4</v>
+      </c>
+      <c r="B17">
+        <v>10</v>
+      </c>
+      <c r="C17" t="s">
+        <v>7</v>
+      </c>
+      <c r="D17">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" t="s">
+        <v>4</v>
+      </c>
+      <c r="B18">
+        <v>4</v>
+      </c>
+      <c r="C18" t="s">
+        <v>5</v>
+      </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" t="s">
+        <v>4</v>
+      </c>
+      <c r="B19">
+        <v>5</v>
+      </c>
+      <c r="C19" t="s">
+        <v>5</v>
+      </c>
+      <c r="D19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" t="s">
+        <v>4</v>
+      </c>
+      <c r="B20">
+        <v>6</v>
+      </c>
+      <c r="C20" t="s">
+        <v>5</v>
+      </c>
+      <c r="D20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" t="s">
+        <v>4</v>
+      </c>
+      <c r="B21">
+        <v>7</v>
+      </c>
+      <c r="C21" t="s">
+        <v>5</v>
+      </c>
+      <c r="D21">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" t="s">
+        <v>4</v>
+      </c>
+      <c r="B22" s="2">
+        <v>8</v>
+      </c>
+      <c r="C22" t="s">
+        <v>5</v>
+      </c>
+      <c r="D22">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" t="s">
+        <v>4</v>
+      </c>
+      <c r="B23">
+        <v>9</v>
+      </c>
+      <c r="C23" t="s">
+        <v>5</v>
+      </c>
+      <c r="D23">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24" t="s">
+        <v>4</v>
+      </c>
+      <c r="B24">
+        <v>10</v>
+      </c>
+      <c r="C24" t="s">
+        <v>5</v>
+      </c>
+      <c r="D24">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="A25" t="s">
+        <v>4</v>
+      </c>
+      <c r="B25">
+        <v>4</v>
+      </c>
+      <c r="C25" t="s">
+        <v>6</v>
+      </c>
+      <c r="D25">
+        <v>0.28000000000000003</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
+      <c r="A26" t="s">
+        <v>4</v>
+      </c>
+      <c r="B26">
+        <v>5</v>
+      </c>
+      <c r="C26" t="s">
+        <v>6</v>
+      </c>
+      <c r="D26">
+        <v>0.35</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
+      <c r="A27" t="s">
+        <v>4</v>
+      </c>
+      <c r="B27">
+        <v>6</v>
+      </c>
+      <c r="C27" t="s">
+        <v>6</v>
+      </c>
+      <c r="D27">
+        <v>0.42</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
+      <c r="A28" t="s">
+        <v>4</v>
+      </c>
+      <c r="B28">
+        <v>7</v>
+      </c>
+      <c r="C28" t="s">
+        <v>6</v>
+      </c>
+      <c r="D28">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
+      <c r="A29" t="s">
+        <v>4</v>
+      </c>
+      <c r="B29">
+        <v>8</v>
+      </c>
+      <c r="C29" t="s">
+        <v>6</v>
+      </c>
+      <c r="D29">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4">
+      <c r="A30" t="s">
+        <v>4</v>
+      </c>
+      <c r="B30">
+        <v>9</v>
+      </c>
+      <c r="C30" t="s">
+        <v>6</v>
+      </c>
+      <c r="D30">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4">
+      <c r="A31" t="s">
+        <v>4</v>
+      </c>
+      <c r="B31">
+        <v>10</v>
+      </c>
+      <c r="C31" t="s">
+        <v>6</v>
+      </c>
+      <c r="D31">
+        <v>0.5</v>
+      </c>
+    </row>
   </sheetData>
+  <sortState ref="A11:D31">
+    <sortCondition ref="C11:C31"/>
+    <sortCondition ref="A11:A31"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
   <drawing r:id="rId2"/>

</xml_diff>

<commit_message>
Se deja fileScan2Times.xlsx como estaba antes del fin de semana pasado. Nosotros el fin de semana pasado habíamos hecho pruebas que invalidaban el análisis del File Scan hecho sobre una traza 2 veces con estrategia FIFO.
La primera vez habíamos obtenido, correctamente, que FIFO daba un HitRate de 0% para una cantidad de bloques menor a la cantidad de páginas en la traza. El fin de semana pasado nos daba un HitRate mayor a 0% para esos casos porque estabamos trabajando con un PAUSE_BETWEEN_REFERENCES igual a 0 en DemoStrategy.
</commit_message>
<xml_diff>
--- a/tp2/resultados/fileScan2Times.xlsx
+++ b/tp2/resultados/fileScan2Times.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>#FRAMES</t>
   </si>
@@ -29,33 +29,13 @@
   <si>
     <t>FIFO</t>
   </si>
-  <si>
-    <t>fileScan2Times.txt</t>
-  </si>
-  <si>
-    <t>LRUReplacementStrategy</t>
-  </si>
-  <si>
-    <t>MRUReplacementStrategy</t>
-  </si>
-  <si>
-    <t>FIFOReplacementStrategy</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <fonts count="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -83,10 +63,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -122,9 +101,9 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="0.12141740791315186"/>
-          <c:y val="3.9058996253436652E-2"/>
+          <c:y val="3.9058996253436659E-2"/>
           <c:w val="0.75458577402297966"/>
-          <c:h val="0.77207238277273382"/>
+          <c:h val="0.77207238277273393"/>
         </c:manualLayout>
       </c:layout>
       <c:line3DChart>
@@ -376,12 +355,13 @@
           </c:val>
           <c:bubble3D val="1"/>
         </c:ser>
-        <c:axId val="79075200"/>
-        <c:axId val="53616640"/>
-        <c:axId val="79054144"/>
+        <c:dLbls/>
+        <c:axId val="69686784"/>
+        <c:axId val="79164160"/>
+        <c:axId val="100932672"/>
       </c:line3DChart>
       <c:catAx>
-        <c:axId val="79075200"/>
+        <c:axId val="69686784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -407,14 +387,14 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="53616640"/>
+        <c:crossAx val="79164160"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="53616640"/>
+        <c:axId val="79164160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -440,12 +420,12 @@
         </c:title>
         <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="79075200"/>
+        <c:crossAx val="69686784"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:serAx>
-        <c:axId val="79054144"/>
+        <c:axId val="100932672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -453,8 +433,7 @@
         <c:axPos val="b"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="53616640"/>
-        <c:crosses val="autoZero"/>
+        <c:crossAx val="79164160"/>
       </c:serAx>
     </c:plotArea>
     <c:legend>
@@ -463,194 +442,6 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="span"/>
-  </c:chart>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="es-AR"/>
-  <c:chart>
-    <c:view3D>
-      <c:rotX val="20"/>
-      <c:rotY val="10"/>
-      <c:perspective val="0"/>
-    </c:view3D>
-    <c:plotArea>
-      <c:layout>
-        <c:manualLayout>
-          <c:layoutTarget val="inner"/>
-          <c:xMode val="edge"/>
-          <c:yMode val="edge"/>
-          <c:x val="0.13138511651828899"/>
-          <c:y val="4.824724999262732E-2"/>
-          <c:w val="0.74695436009845584"/>
-          <c:h val="0.86941307617446695"/>
-        </c:manualLayout>
-      </c:layout>
-      <c:line3DChart>
-        <c:grouping val="standard"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:v>FIFO</c:v>
-          </c:tx>
-          <c:val>
-            <c:numRef>
-              <c:f>Hoja1!$D$11:$D$17</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>0.21</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.21</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.42</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.5</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.5</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.5</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.5</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:v>LRU</c:v>
-          </c:tx>
-          <c:val>
-            <c:numRef>
-              <c:f>Hoja1!$D$18:$D$24</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.5</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.5</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.5</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.5</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:v>MRU</c:v>
-          </c:tx>
-          <c:val>
-            <c:numRef>
-              <c:f>Hoja1!$D$25:$D$31</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>0.28000000000000003</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.35</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.42</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.5</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.5</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.5</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.5</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:axId val="74438528"/>
-        <c:axId val="74461952"/>
-        <c:axId val="80919616"/>
-      </c:line3DChart>
-      <c:catAx>
-        <c:axId val="74438528"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:axPos val="b"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="74461952"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="74461952"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:axPos val="l"/>
-        <c:majorGridlines/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="74438528"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-      <c:serAx>
-        <c:axId val="80919616"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:axPos val="b"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="74461952"/>
-      </c:serAx>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:layout/>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
@@ -664,15 +455,15 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>4</xdr:row>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>962025</xdr:colOff>
+      <xdr:row>1</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>685800</xdr:colOff>
-      <xdr:row>26</xdr:row>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>23</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -687,36 +478,6 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>733424</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>761999</xdr:colOff>
-      <xdr:row>53</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="3 Gráfico"/>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1023,10 +784,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D31"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="E34" sqref="E34"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N22" sqref="N22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1147,305 +908,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
-      <c r="A11" t="s">
-        <v>4</v>
-      </c>
-      <c r="B11">
-        <v>4</v>
-      </c>
-      <c r="C11" t="s">
-        <v>7</v>
-      </c>
-      <c r="D11">
-        <v>0.21</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
-      <c r="A12" t="s">
-        <v>4</v>
-      </c>
-      <c r="B12">
-        <v>5</v>
-      </c>
-      <c r="C12" t="s">
-        <v>7</v>
-      </c>
-      <c r="D12">
-        <v>0.21</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4">
-      <c r="A13" t="s">
-        <v>4</v>
-      </c>
-      <c r="B13">
-        <v>6</v>
-      </c>
-      <c r="C13" t="s">
-        <v>7</v>
-      </c>
-      <c r="D13">
-        <v>0.42</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4">
-      <c r="A14" t="s">
-        <v>4</v>
-      </c>
-      <c r="B14">
-        <v>7</v>
-      </c>
-      <c r="C14" t="s">
-        <v>7</v>
-      </c>
-      <c r="D14">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4">
-      <c r="A15" t="s">
-        <v>4</v>
-      </c>
-      <c r="B15">
-        <v>8</v>
-      </c>
-      <c r="C15" t="s">
-        <v>7</v>
-      </c>
-      <c r="D15">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4">
-      <c r="A16" t="s">
-        <v>4</v>
-      </c>
-      <c r="B16">
-        <v>9</v>
-      </c>
-      <c r="C16" t="s">
-        <v>7</v>
-      </c>
-      <c r="D16">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4">
-      <c r="A17" t="s">
-        <v>4</v>
-      </c>
-      <c r="B17">
-        <v>10</v>
-      </c>
-      <c r="C17" t="s">
-        <v>7</v>
-      </c>
-      <c r="D17">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4">
-      <c r="A18" t="s">
-        <v>4</v>
-      </c>
-      <c r="B18">
-        <v>4</v>
-      </c>
-      <c r="C18" t="s">
-        <v>5</v>
-      </c>
-      <c r="D18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4">
-      <c r="A19" t="s">
-        <v>4</v>
-      </c>
-      <c r="B19">
-        <v>5</v>
-      </c>
-      <c r="C19" t="s">
-        <v>5</v>
-      </c>
-      <c r="D19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4">
-      <c r="A20" t="s">
-        <v>4</v>
-      </c>
-      <c r="B20">
-        <v>6</v>
-      </c>
-      <c r="C20" t="s">
-        <v>5</v>
-      </c>
-      <c r="D20">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4">
-      <c r="A21" t="s">
-        <v>4</v>
-      </c>
-      <c r="B21">
-        <v>7</v>
-      </c>
-      <c r="C21" t="s">
-        <v>5</v>
-      </c>
-      <c r="D21">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4">
-      <c r="A22" t="s">
-        <v>4</v>
-      </c>
-      <c r="B22" s="2">
-        <v>8</v>
-      </c>
-      <c r="C22" t="s">
-        <v>5</v>
-      </c>
-      <c r="D22">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4">
-      <c r="A23" t="s">
-        <v>4</v>
-      </c>
-      <c r="B23">
-        <v>9</v>
-      </c>
-      <c r="C23" t="s">
-        <v>5</v>
-      </c>
-      <c r="D23">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4">
-      <c r="A24" t="s">
-        <v>4</v>
-      </c>
-      <c r="B24">
-        <v>10</v>
-      </c>
-      <c r="C24" t="s">
-        <v>5</v>
-      </c>
-      <c r="D24">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4">
-      <c r="A25" t="s">
-        <v>4</v>
-      </c>
-      <c r="B25">
-        <v>4</v>
-      </c>
-      <c r="C25" t="s">
-        <v>6</v>
-      </c>
-      <c r="D25">
-        <v>0.28000000000000003</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4">
-      <c r="A26" t="s">
-        <v>4</v>
-      </c>
-      <c r="B26">
-        <v>5</v>
-      </c>
-      <c r="C26" t="s">
-        <v>6</v>
-      </c>
-      <c r="D26">
-        <v>0.35</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4">
-      <c r="A27" t="s">
-        <v>4</v>
-      </c>
-      <c r="B27">
-        <v>6</v>
-      </c>
-      <c r="C27" t="s">
-        <v>6</v>
-      </c>
-      <c r="D27">
-        <v>0.42</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4">
-      <c r="A28" t="s">
-        <v>4</v>
-      </c>
-      <c r="B28">
-        <v>7</v>
-      </c>
-      <c r="C28" t="s">
-        <v>6</v>
-      </c>
-      <c r="D28">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4">
-      <c r="A29" t="s">
-        <v>4</v>
-      </c>
-      <c r="B29">
-        <v>8</v>
-      </c>
-      <c r="C29" t="s">
-        <v>6</v>
-      </c>
-      <c r="D29">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4">
-      <c r="A30" t="s">
-        <v>4</v>
-      </c>
-      <c r="B30">
-        <v>9</v>
-      </c>
-      <c r="C30" t="s">
-        <v>6</v>
-      </c>
-      <c r="D30">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4">
-      <c r="A31" t="s">
-        <v>4</v>
-      </c>
-      <c r="B31">
-        <v>10</v>
-      </c>
-      <c r="C31" t="s">
-        <v>6</v>
-      </c>
-      <c r="D31">
-        <v>0.5</v>
-      </c>
-    </row>
   </sheetData>
-  <sortState ref="A11:D31">
-    <sortCondition ref="C11:C31"/>
-    <sortCondition ref="A11:A31"/>
-  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
   <drawing r:id="rId2"/>

</xml_diff>